<commit_message>
fix(libs): non assessable nodes
</commit_message>
<xml_diff>
--- a/tools/swift-cscf-v2025v1.0.xlsx
+++ b/tools/swift-cscf-v2025v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/BaillCe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CD34EB-9F6D-1541-AF14-A95CF6F39B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEF05B3-E600-504C-927D-79B96CF72116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29920" windowHeight="18680" activeTab="1" xr2:uid="{49ED024B-26A8-8540-A8C6-6290589ABC82}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{49ED024B-26A8-8540-A8C6-6290589ABC82}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>urn:intuitem:risk:framework:swift-cscf-v2025</t>
+  </si>
+  <si>
+    <t>Swift Customer Security Controls Framework v2025 - outline</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -811,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0FB091-DB8B-424C-8CA7-8AA41036D39B}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -836,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -868,7 +871,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,7 +927,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -948,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9C3373-09B8-FD49-B816-2560F9A17BDE}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="132" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView topLeftCell="A22" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,9 +995,6 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
@@ -1104,9 +1104,6 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="B11" s="6">
         <v>2</v>
       </c>
@@ -1160,9 +1157,6 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="B15" s="6">
         <v>2</v>
       </c>

</xml_diff>